<commit_message>
add the statistic of std
</commit_message>
<xml_diff>
--- a/Experiment_Results(AutoRecovered).xlsx
+++ b/Experiment_Results(AutoRecovered).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xutao/PycharmProjects/Network_tomography/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB827ACE-345D-1A4C-BEEB-8F8872C24AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AC1254-5871-7740-A05A-ADC85E31FF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48760" yWindow="1780" windowWidth="26880" windowHeight="16440" activeTab="1" xr2:uid="{364D682F-7B04-A048-A598-7CE26482F535}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="32120" windowHeight="20380" activeTab="2" xr2:uid="{364D682F-7B04-A048-A598-7CE26482F535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -610,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0D411F-4F63-514D-938F-FE1D43ED4FCD}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -1250,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F457393F-D1A3-0148-8982-D629C1124A02}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2144,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81467EFA-C694-4D44-8B73-934D56799AE2}">
   <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="151" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="151" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>